<commit_message>
🗃️ (whole app) : Create new mutations and an script for data management
</commit_message>
<xml_diff>
--- a/Downloads/Liste de mots allemands 2021-2022.xlsx
+++ b/Downloads/Liste de mots allemands 2021-2022.xlsx
@@ -8,17 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pierr\IT-Development\Nuxt-Projects\my-nuxt3-app-01\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4285B12-7BF7-48BC-B90D-96F2C6FDD6F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D6F57A-A0DD-45E6-86AA-8BA24A83344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1000,10 +1010,10 @@
   <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E65" sqref="E65"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>